<commit_message>
prueba tecnica de nuxiba
</commit_message>
<xml_diff>
--- a/Prueba_2/DatosPracticaSQL.xlsx
+++ b/Prueba_2/DatosPracticaSQL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rokoko/Desktop/Logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/10e1a1b1e026d403/Escritorio/testdevfrontjr/Prueba_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D48591-0467-9242-9FBC-3C0DC525BE08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D8D48591-0467-9242-9FBC-3C0DC525BE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE703A99-60A9-44A1-87FB-FD461F76D6EE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22500" xr2:uid="{12404B0B-7D3E-44C7-92CA-59F8C1921DED}"/>
+    <workbookView xWindow="38280" yWindow="3150" windowWidth="29040" windowHeight="15840" xr2:uid="{12404B0B-7D3E-44C7-92CA-59F8C1921DED}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoLogDial" sheetId="2" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -501,13 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,9 +519,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -566,7 +559,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -672,7 +665,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -814,7 +807,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -825,19 +818,19 @@
   <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -854,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>197463</v>
       </c>
@@ -864,14 +857,14 @@
       <c r="C2" s="3">
         <v>60</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2">
         <v>8000000001</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>197464</v>
       </c>
@@ -881,14 +874,14 @@
       <c r="C3" s="3">
         <v>60</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3">
         <v>8000000002</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>197465</v>
       </c>
@@ -898,14 +891,14 @@
       <c r="C4" s="3">
         <v>240</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>8000000003</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>197466</v>
       </c>
@@ -915,14 +908,14 @@
       <c r="C5" s="3">
         <v>60</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>8000000004</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>197467</v>
       </c>
@@ -932,14 +925,14 @@
       <c r="C6" s="3">
         <v>60</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>8000000005</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>197468</v>
       </c>
@@ -949,14 +942,14 @@
       <c r="C7" s="3">
         <v>60</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>8000000006</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>197469</v>
       </c>
@@ -966,14 +959,14 @@
       <c r="C8" s="3">
         <v>60</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>8000000007</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>197470</v>
       </c>
@@ -983,14 +976,14 @@
       <c r="C9" s="3">
         <v>120</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>8000000008</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>197471</v>
       </c>
@@ -1000,14 +993,14 @@
       <c r="C10" s="3">
         <v>60</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>8000000009</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>197472</v>
       </c>
@@ -1017,14 +1010,14 @@
       <c r="C11" s="3">
         <v>60</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11">
         <v>8000000010</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>197473</v>
       </c>
@@ -1034,14 +1027,14 @@
       <c r="C12" s="3">
         <v>120</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12">
         <v>8000000011</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>197474</v>
       </c>
@@ -1051,14 +1044,14 @@
       <c r="C13" s="3">
         <v>60</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13">
         <v>8000000012</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>197475</v>
       </c>
@@ -1068,14 +1061,14 @@
       <c r="C14" s="3">
         <v>60</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14">
         <v>8000000013</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>197476</v>
       </c>
@@ -1085,14 +1078,14 @@
       <c r="C15" s="3">
         <v>60</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15">
         <v>8000000014</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>197477</v>
       </c>
@@ -1102,14 +1095,14 @@
       <c r="C16" s="3">
         <v>120</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16">
         <v>8000000015</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>197478</v>
       </c>
@@ -1119,14 +1112,14 @@
       <c r="C17" s="3">
         <v>60</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17">
         <v>8000000016</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>197479</v>
       </c>
@@ -1136,14 +1129,14 @@
       <c r="C18" s="3">
         <v>60</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18">
         <v>8000000017</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>197480</v>
       </c>
@@ -1153,14 +1146,14 @@
       <c r="C19" s="3">
         <v>60</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19">
         <v>8000000018</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>197481</v>
       </c>
@@ -1170,14 +1163,14 @@
       <c r="C20" s="3">
         <v>180</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20">
         <v>8000000019</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>197482</v>
       </c>
@@ -1187,14 +1180,14 @@
       <c r="C21" s="3">
         <v>120</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21">
         <v>8000000020</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>197483</v>
       </c>
@@ -1204,14 +1197,14 @@
       <c r="C22" s="3">
         <v>60</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22">
         <v>8000000021</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>197484</v>
       </c>
@@ -1221,14 +1214,14 @@
       <c r="C23" s="3">
         <v>60</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23">
         <v>8000000022</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>197485</v>
       </c>
@@ -1238,14 +1231,14 @@
       <c r="C24" s="3">
         <v>60</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24">
         <v>8000000023</v>
       </c>
       <c r="E24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>197486</v>
       </c>
@@ -1255,14 +1248,14 @@
       <c r="C25" s="3">
         <v>120</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25">
         <v>8000000024</v>
       </c>
       <c r="E25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>197487</v>
       </c>
@@ -1272,14 +1265,14 @@
       <c r="C26" s="3">
         <v>60</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26">
         <v>8000000025</v>
       </c>
       <c r="E26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>197488</v>
       </c>
@@ -1289,14 +1282,14 @@
       <c r="C27" s="3">
         <v>60</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27">
         <v>8000000026</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>197489</v>
       </c>
@@ -1306,14 +1299,14 @@
       <c r="C28" s="3">
         <v>120</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28">
         <v>8000000027</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>197490</v>
       </c>
@@ -1323,14 +1316,14 @@
       <c r="C29" s="3">
         <v>60</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29">
         <v>8000000028</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>197491</v>
       </c>
@@ -1340,14 +1333,14 @@
       <c r="C30" s="3">
         <v>76</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30">
         <v>8000000029</v>
       </c>
       <c r="E30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>197492</v>
       </c>
@@ -1357,14 +1350,14 @@
       <c r="C31" s="3">
         <v>60</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31">
         <v>8000000030</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>197493</v>
       </c>
@@ -1374,14 +1367,14 @@
       <c r="C32" s="3">
         <v>60</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32">
         <v>8000000031</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>197494</v>
       </c>
@@ -1391,14 +1384,14 @@
       <c r="C33" s="3">
         <v>60</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33">
         <v>8000000032</v>
       </c>
       <c r="E33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>197495</v>
       </c>
@@ -1408,14 +1401,14 @@
       <c r="C34" s="3">
         <v>60</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34">
         <v>8000000033</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>197496</v>
       </c>
@@ -1425,14 +1418,14 @@
       <c r="C35" s="3">
         <v>240</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35">
         <v>8000000034</v>
       </c>
       <c r="E35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>197497</v>
       </c>
@@ -1442,14 +1435,14 @@
       <c r="C36" s="3">
         <v>60</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36">
         <v>8000000035</v>
       </c>
       <c r="E36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>197498</v>
       </c>
@@ -1459,14 +1452,14 @@
       <c r="C37" s="3">
         <v>240</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37">
         <v>8000000036</v>
       </c>
       <c r="E37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>197499</v>
       </c>
@@ -1476,14 +1469,14 @@
       <c r="C38" s="3">
         <v>120</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38">
         <v>8000000037</v>
       </c>
       <c r="E38" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>197500</v>
       </c>
@@ -1493,14 +1486,14 @@
       <c r="C39" s="3">
         <v>95</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39">
         <v>8000000038</v>
       </c>
       <c r="E39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>197501</v>
       </c>
@@ -1510,14 +1503,14 @@
       <c r="C40" s="3">
         <v>60</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40">
         <v>8000000039</v>
       </c>
       <c r="E40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>197502</v>
       </c>
@@ -1527,14 +1520,14 @@
       <c r="C41" s="3">
         <v>60</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41">
         <v>8000000040</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>197503</v>
       </c>
@@ -1544,14 +1537,14 @@
       <c r="C42" s="3">
         <v>360</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42">
         <v>8000000041</v>
       </c>
       <c r="E42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>197504</v>
       </c>
@@ -1561,14 +1554,14 @@
       <c r="C43" s="3">
         <v>60</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43">
         <v>8000000042</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>197505</v>
       </c>
@@ -1578,14 +1571,14 @@
       <c r="C44" s="3">
         <v>60</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44">
         <v>8000000043</v>
       </c>
       <c r="E44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>197506</v>
       </c>
@@ -1595,14 +1588,14 @@
       <c r="C45" s="3">
         <v>60</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45">
         <v>8000000044</v>
       </c>
       <c r="E45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>197507</v>
       </c>
@@ -1612,14 +1605,14 @@
       <c r="C46" s="3">
         <v>120</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46">
         <v>8000000045</v>
       </c>
       <c r="E46" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>197508</v>
       </c>
@@ -1629,14 +1622,14 @@
       <c r="C47" s="3">
         <v>60</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47">
         <v>8000000046</v>
       </c>
       <c r="E47" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>197509</v>
       </c>
@@ -1646,14 +1639,14 @@
       <c r="C48" s="3">
         <v>60</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48">
         <v>8000000047</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>197510</v>
       </c>
@@ -1663,14 +1656,14 @@
       <c r="C49" s="3">
         <v>120</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49">
         <v>8000000048</v>
       </c>
       <c r="E49" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>197511</v>
       </c>
@@ -1680,14 +1673,14 @@
       <c r="C50" s="3">
         <v>120</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50">
         <v>8000000049</v>
       </c>
       <c r="E50" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>197512</v>
       </c>
@@ -1697,14 +1690,14 @@
       <c r="C51" s="3">
         <v>60</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51">
         <v>8000000050</v>
       </c>
       <c r="E51" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>197513</v>
       </c>
@@ -1714,14 +1707,14 @@
       <c r="C52" s="3">
         <v>85</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52">
         <v>8000000051</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>197514</v>
       </c>
@@ -1731,14 +1724,14 @@
       <c r="C53" s="3">
         <v>60</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53">
         <v>8000000052</v>
       </c>
       <c r="E53" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>197515</v>
       </c>
@@ -1748,14 +1741,14 @@
       <c r="C54" s="3">
         <v>60</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54">
         <v>8000000053</v>
       </c>
       <c r="E54" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>197516</v>
       </c>
@@ -1765,14 +1758,14 @@
       <c r="C55" s="3">
         <v>120</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55">
         <v>8000000054</v>
       </c>
       <c r="E55" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>197517</v>
       </c>
@@ -1782,14 +1775,14 @@
       <c r="C56" s="3">
         <v>120</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56">
         <v>8000000055</v>
       </c>
       <c r="E56" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>197518</v>
       </c>
@@ -1799,14 +1792,14 @@
       <c r="C57" s="3">
         <v>240</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57">
         <v>8000000056</v>
       </c>
       <c r="E57" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>197519</v>
       </c>
@@ -1816,14 +1809,14 @@
       <c r="C58" s="3">
         <v>60</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58">
         <v>8000000057</v>
       </c>
       <c r="E58" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>197520</v>
       </c>
@@ -1833,14 +1826,14 @@
       <c r="C59" s="3">
         <v>180</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59">
         <v>8000000058</v>
       </c>
       <c r="E59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>197521</v>
       </c>
@@ -1850,14 +1843,14 @@
       <c r="C60" s="3">
         <v>180</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D60">
         <v>8000000059</v>
       </c>
       <c r="E60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>197522</v>
       </c>
@@ -1867,14 +1860,14 @@
       <c r="C61" s="3">
         <v>120</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D61">
         <v>8000000060</v>
       </c>
       <c r="E61" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>197523</v>
       </c>
@@ -1884,14 +1877,14 @@
       <c r="C62" s="3">
         <v>60</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62">
         <v>8000000061</v>
       </c>
       <c r="E62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>197524</v>
       </c>
@@ -1901,14 +1894,14 @@
       <c r="C63" s="3">
         <v>60</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D63">
         <v>8000000062</v>
       </c>
       <c r="E63" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>197525</v>
       </c>
@@ -1918,14 +1911,14 @@
       <c r="C64" s="3">
         <v>120</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64">
         <v>8000000063</v>
       </c>
       <c r="E64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>197526</v>
       </c>
@@ -1935,14 +1928,14 @@
       <c r="C65" s="3">
         <v>60</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65">
         <v>8000000064</v>
       </c>
       <c r="E65" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>197527</v>
       </c>
@@ -1952,14 +1945,14 @@
       <c r="C66" s="3">
         <v>60</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66">
         <v>8000000065</v>
       </c>
       <c r="E66" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>197528</v>
       </c>
@@ -1969,14 +1962,14 @@
       <c r="C67" s="3">
         <v>60</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67">
         <v>8000000066</v>
       </c>
       <c r="E67" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>197529</v>
       </c>
@@ -1986,14 +1979,14 @@
       <c r="C68" s="3">
         <v>60</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68">
         <v>8000000067</v>
       </c>
       <c r="E68" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>197530</v>
       </c>
@@ -2003,14 +1996,14 @@
       <c r="C69" s="3">
         <v>60</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69">
         <v>8000000068</v>
       </c>
       <c r="E69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>197531</v>
       </c>
@@ -2020,14 +2013,14 @@
       <c r="C70" s="3">
         <v>60</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70">
         <v>8000000069</v>
       </c>
       <c r="E70" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>197532</v>
       </c>
@@ -2037,14 +2030,14 @@
       <c r="C71" s="3">
         <v>60</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71">
         <v>8000000070</v>
       </c>
       <c r="E71" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>197533</v>
       </c>
@@ -2054,14 +2047,14 @@
       <c r="C72" s="3">
         <v>60</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72">
         <v>8000000071</v>
       </c>
       <c r="E72" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>197534</v>
       </c>
@@ -2071,14 +2064,14 @@
       <c r="C73" s="3">
         <v>120</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73">
         <v>8000000072</v>
       </c>
       <c r="E73" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>197535</v>
       </c>
@@ -2088,14 +2081,14 @@
       <c r="C74" s="3">
         <v>60</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74">
         <v>8000000073</v>
       </c>
       <c r="E74" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>197536</v>
       </c>
@@ -2105,14 +2098,14 @@
       <c r="C75" s="3">
         <v>60</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75">
         <v>8000000074</v>
       </c>
       <c r="E75" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>197537</v>
       </c>
@@ -2122,14 +2115,14 @@
       <c r="C76" s="3">
         <v>60</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76">
         <v>8000000075</v>
       </c>
       <c r="E76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>197538</v>
       </c>
@@ -2139,14 +2132,14 @@
       <c r="C77" s="3">
         <v>120</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77">
         <v>8000000076</v>
       </c>
       <c r="E77" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>197539</v>
       </c>
@@ -2156,14 +2149,14 @@
       <c r="C78" s="3">
         <v>60</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78">
         <v>8000000077</v>
       </c>
       <c r="E78" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>197540</v>
       </c>
@@ -2173,14 +2166,14 @@
       <c r="C79" s="3">
         <v>60</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79">
         <v>8000000078</v>
       </c>
       <c r="E79" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>197541</v>
       </c>
@@ -2190,14 +2183,14 @@
       <c r="C80" s="3">
         <v>86</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80">
         <v>8000000079</v>
       </c>
       <c r="E80" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>197542</v>
       </c>
@@ -2207,14 +2200,14 @@
       <c r="C81" s="3">
         <v>120</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81">
         <v>8000000080</v>
       </c>
       <c r="E81" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>197543</v>
       </c>
@@ -2224,14 +2217,14 @@
       <c r="C82" s="3">
         <v>120</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82">
         <v>8000000081</v>
       </c>
       <c r="E82" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>197544</v>
       </c>
@@ -2241,14 +2234,14 @@
       <c r="C83" s="3">
         <v>60</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83">
         <v>8000000082</v>
       </c>
       <c r="E83" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>197545</v>
       </c>
@@ -2258,14 +2251,14 @@
       <c r="C84" s="3">
         <v>77</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84">
         <v>8000000083</v>
       </c>
       <c r="E84" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>197546</v>
       </c>
@@ -2275,14 +2268,14 @@
       <c r="C85" s="3">
         <v>60</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85">
         <v>8000000084</v>
       </c>
       <c r="E85" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>197547</v>
       </c>
@@ -2292,14 +2285,14 @@
       <c r="C86" s="3">
         <v>60</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86">
         <v>8000000085</v>
       </c>
       <c r="E86" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>197548</v>
       </c>
@@ -2309,14 +2302,14 @@
       <c r="C87" s="3">
         <v>120</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D87">
         <v>8000000086</v>
       </c>
       <c r="E87" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>197549</v>
       </c>
@@ -2326,14 +2319,14 @@
       <c r="C88" s="3">
         <v>180</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D88">
         <v>8000000087</v>
       </c>
       <c r="E88" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>197550</v>
       </c>
@@ -2343,14 +2336,14 @@
       <c r="C89" s="3">
         <v>180</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D89">
         <v>8000000088</v>
       </c>
       <c r="E89" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>197551</v>
       </c>
@@ -2360,14 +2353,14 @@
       <c r="C90" s="3">
         <v>60</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90">
         <v>8000000089</v>
       </c>
       <c r="E90" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>197552</v>
       </c>
@@ -2377,14 +2370,14 @@
       <c r="C91" s="3">
         <v>60</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D91">
         <v>8000000090</v>
       </c>
       <c r="E91" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>197553</v>
       </c>
@@ -2394,14 +2387,14 @@
       <c r="C92" s="3">
         <v>60</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92">
         <v>8000000091</v>
       </c>
       <c r="E92" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>197554</v>
       </c>
@@ -2411,14 +2404,14 @@
       <c r="C93" s="3">
         <v>60</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D93">
         <v>8000000092</v>
       </c>
       <c r="E93" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>197555</v>
       </c>
@@ -2428,14 +2421,14 @@
       <c r="C94" s="3">
         <v>60</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94">
         <v>8000000093</v>
       </c>
       <c r="E94" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>197556</v>
       </c>
@@ -2445,14 +2438,14 @@
       <c r="C95" s="3">
         <v>180</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D95">
         <v>8000000094</v>
       </c>
       <c r="E95" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>197557</v>
       </c>
@@ -2462,14 +2455,14 @@
       <c r="C96" s="3">
         <v>60</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96">
         <v>8000000095</v>
       </c>
       <c r="E96" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>197558</v>
       </c>
@@ -2479,14 +2472,14 @@
       <c r="C97" s="3">
         <v>196</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97">
         <v>8000000096</v>
       </c>
       <c r="E97" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>197559</v>
       </c>
@@ -2496,14 +2489,14 @@
       <c r="C98" s="3">
         <v>60</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98">
         <v>8000000097</v>
       </c>
       <c r="E98" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>197560</v>
       </c>
@@ -2513,14 +2506,14 @@
       <c r="C99" s="3">
         <v>60</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D99">
         <v>8000000098</v>
       </c>
       <c r="E99" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>197561</v>
       </c>
@@ -2530,14 +2523,14 @@
       <c r="C100" s="3">
         <v>60</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100">
         <v>8000000099</v>
       </c>
       <c r="E100" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>197562</v>
       </c>
@@ -2547,14 +2540,14 @@
       <c r="C101" s="3">
         <v>60</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101">
         <v>8000000100</v>
       </c>
       <c r="E101" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>197563</v>
       </c>
@@ -2564,14 +2557,14 @@
       <c r="C102" s="3">
         <v>60</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D102">
         <v>8000000101</v>
       </c>
       <c r="E102" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>197564</v>
       </c>
@@ -2581,14 +2574,14 @@
       <c r="C103" s="3">
         <v>60</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D103">
         <v>8000000102</v>
       </c>
       <c r="E103" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>197565</v>
       </c>
@@ -2598,14 +2591,14 @@
       <c r="C104" s="3">
         <v>60</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D104">
         <v>8000000103</v>
       </c>
       <c r="E104" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>197566</v>
       </c>
@@ -2615,14 +2608,14 @@
       <c r="C105" s="3">
         <v>120</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D105">
         <v>8000000104</v>
       </c>
       <c r="E105" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>197567</v>
       </c>
@@ -2632,14 +2625,14 @@
       <c r="C106" s="3">
         <v>180</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D106">
         <v>8000000105</v>
       </c>
       <c r="E106" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>197568</v>
       </c>
@@ -2649,14 +2642,14 @@
       <c r="C107" s="3">
         <v>60</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D107">
         <v>8000000106</v>
       </c>
       <c r="E107" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>197569</v>
       </c>
@@ -2666,14 +2659,14 @@
       <c r="C108" s="3">
         <v>60</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D108">
         <v>8000000107</v>
       </c>
       <c r="E108" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>197570</v>
       </c>
@@ -2683,14 +2676,14 @@
       <c r="C109" s="3">
         <v>60</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D109">
         <v>8000000108</v>
       </c>
       <c r="E109" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>197571</v>
       </c>
@@ -2700,14 +2693,14 @@
       <c r="C110" s="3">
         <v>180</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D110">
         <v>8000000109</v>
       </c>
       <c r="E110" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>197572</v>
       </c>
@@ -2717,14 +2710,14 @@
       <c r="C111" s="3">
         <v>60</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D111">
         <v>8000000110</v>
       </c>
       <c r="E111" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>197573</v>
       </c>
@@ -2734,14 +2727,14 @@
       <c r="C112" s="3">
         <v>60</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D112">
         <v>8000000111</v>
       </c>
       <c r="E112" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>197574</v>
       </c>
@@ -2751,14 +2744,14 @@
       <c r="C113" s="3">
         <v>60</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D113">
         <v>8000000112</v>
       </c>
       <c r="E113" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>197575</v>
       </c>
@@ -2768,14 +2761,14 @@
       <c r="C114" s="3">
         <v>60</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D114">
         <v>8000000113</v>
       </c>
       <c r="E114" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>197576</v>
       </c>
@@ -2785,14 +2778,14 @@
       <c r="C115" s="3">
         <v>60</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D115">
         <v>8000000114</v>
       </c>
       <c r="E115" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>197577</v>
       </c>
@@ -2802,14 +2795,14 @@
       <c r="C116" s="3">
         <v>60</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D116">
         <v>8000000115</v>
       </c>
       <c r="E116" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>197578</v>
       </c>
@@ -2819,14 +2812,14 @@
       <c r="C117" s="3">
         <v>60</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D117">
         <v>8000000116</v>
       </c>
       <c r="E117" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>197579</v>
       </c>
@@ -2836,14 +2829,14 @@
       <c r="C118" s="3">
         <v>60</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D118">
         <v>8000000117</v>
       </c>
       <c r="E118" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>197580</v>
       </c>
@@ -2853,14 +2846,14 @@
       <c r="C119" s="3">
         <v>240</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D119">
         <v>8000000118</v>
       </c>
       <c r="E119" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>197581</v>
       </c>
@@ -2870,14 +2863,14 @@
       <c r="C120" s="3">
         <v>60</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D120">
         <v>8000000119</v>
       </c>
       <c r="E120" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>197582</v>
       </c>
@@ -2887,14 +2880,14 @@
       <c r="C121" s="3">
         <v>60</v>
       </c>
-      <c r="D121" s="6">
+      <c r="D121">
         <v>8000000120</v>
       </c>
       <c r="E121" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>197583</v>
       </c>
@@ -2904,14 +2897,14 @@
       <c r="C122" s="3">
         <v>120</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D122">
         <v>8000000121</v>
       </c>
       <c r="E122" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>197584</v>
       </c>
@@ -2921,14 +2914,14 @@
       <c r="C123" s="3">
         <v>60</v>
       </c>
-      <c r="D123" s="6">
+      <c r="D123">
         <v>8000000122</v>
       </c>
       <c r="E123" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>197585</v>
       </c>
@@ -2938,14 +2931,14 @@
       <c r="C124" s="3">
         <v>60</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D124">
         <v>8000000123</v>
       </c>
       <c r="E124" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>197586</v>
       </c>
@@ -2955,14 +2948,14 @@
       <c r="C125" s="3">
         <v>120</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D125">
         <v>8000000124</v>
       </c>
       <c r="E125" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>197587</v>
       </c>
@@ -2972,14 +2965,14 @@
       <c r="C126" s="3">
         <v>60</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D126">
         <v>8000000125</v>
       </c>
       <c r="E126" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>197588</v>
       </c>
@@ -2989,14 +2982,14 @@
       <c r="C127" s="3">
         <v>60</v>
       </c>
-      <c r="D127" s="6">
+      <c r="D127">
         <v>8000000126</v>
       </c>
       <c r="E127" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>197589</v>
       </c>
@@ -3006,14 +2999,14 @@
       <c r="C128" s="3">
         <v>60</v>
       </c>
-      <c r="D128" s="6">
+      <c r="D128">
         <v>8000000127</v>
       </c>
       <c r="E128" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>197590</v>
       </c>
@@ -3023,27 +3016,27 @@
       <c r="C129" s="3">
         <v>60</v>
       </c>
-      <c r="D129" s="6">
+      <c r="D129">
         <v>8000000128</v>
       </c>
       <c r="E129" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>197591</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B130" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C130" s="9">
+      <c r="C130" s="3">
         <v>120</v>
       </c>
-      <c r="D130" s="10">
+      <c r="D130">
         <v>8000000129</v>
       </c>
-      <c r="E130" s="7" t="s">
+      <c r="E130" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3061,12 +3054,12 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3074,7 +3067,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3082,7 +3075,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3090,7 +3083,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>

</xml_diff>